<commit_message>
:sparkles: Added URP and Started Custom shader
</commit_message>
<xml_diff>
--- a/docs/DTT-Test-Hour-Log-1.xlsx
+++ b/docs/DTT-Test-Hour-Log-1.xlsx
@@ -1,21 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26215"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laurens/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Mazes-for-days\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21E3D882-A776-4890-8C12-B622FA7321B8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="19540"/>
+    <workbookView xWindow="555" yWindow="4290" windowWidth="36690" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DTT Test Hour Log" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -24,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Subject</t>
   </si>
@@ -36,18 +43,6 @@
   </si>
   <si>
     <t>Description</t>
-  </si>
-  <si>
-    <t>Example 1</t>
-  </si>
-  <si>
-    <t>Implementing …</t>
-  </si>
-  <si>
-    <t>Example 2</t>
-  </si>
-  <si>
-    <t>Had some issues with…</t>
   </si>
   <si>
     <t>Total amount of hours</t>
@@ -74,15 +69,33 @@
 Fill in the number of hours that were required to complete the test. Please include every step you took during the proces and include a detailed description of every step. Add reasoning on why you took certain descisions or applied specific techniques. We prefer quality over quantity so take your time with the test and the log.</t>
     </r>
   </si>
+  <si>
+    <t>Generate a Maze</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implementing Hunt and Kill(Drunken walk) algorithm to generate mazes </t>
+  </si>
+  <si>
+    <t>Making UI Functions</t>
+  </si>
+  <si>
+    <t>Made Basic UI Functions hit a snag at clearing the maze but its fixed</t>
+  </si>
+  <si>
+    <t>Made Temporary perfabs</t>
+  </si>
+  <si>
+    <t>Made Quick and dirty test Prefabs and also started to make some extra assets</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -423,8 +436,8 @@
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2"/>
-    <cellStyle name="Standaard 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Standaard 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultPivotStyle="PivotStyleMedium7"/>
@@ -530,7 +543,7 @@
         <xdr:cNvPr id="2" name="image1.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1674,24 +1687,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F2"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="6.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="6.5" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="24.875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.75" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="38.625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="24.8984375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.69921875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.59765625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="38.59765625" style="1" customWidth="1"/>
     <col min="5" max="6" width="6.5" style="1" customWidth="1"/>
     <col min="7" max="251" width="6.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="73.5" customHeight="1">
       <c r="A1" s="20"/>
       <c r="B1" s="21"/>
       <c r="C1" s="21"/>
@@ -1699,9 +1712,9 @@
       <c r="E1" s="11"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="46.5" customHeight="1">
       <c r="A2" s="22" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B2" s="22"/>
       <c r="C2" s="22"/>
@@ -1709,7 +1722,7 @@
       <c r="E2" s="22"/>
       <c r="F2" s="23"/>
     </row>
-    <row r="3" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="17.100000000000001" customHeight="1">
       <c r="A3" s="17" t="s">
         <v>0</v>
       </c>
@@ -1725,47 +1738,55 @@
       <c r="E3" s="3"/>
       <c r="F3" s="5"/>
     </row>
-    <row r="4" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="17.100000000000001" customHeight="1">
       <c r="A4" s="6" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B4" s="18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C4" s="19">
-        <v>42736</v>
+        <v>43952</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="5"/>
     </row>
-    <row r="5" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="17.100000000000001" customHeight="1">
       <c r="A5" s="6" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B5" s="18">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="C5" s="19">
-        <v>42736</v>
+        <v>43952</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="6"/>
-      <c r="B6" s="18"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="16"/>
+    <row r="6" spans="1:6" ht="17.100000000000001" customHeight="1">
+      <c r="A6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="18">
+        <v>1</v>
+      </c>
+      <c r="C6" s="19">
+        <v>43952</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>11</v>
+      </c>
       <c r="E6" s="3"/>
       <c r="F6" s="5"/>
     </row>
-    <row r="7" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="17.100000000000001" customHeight="1">
       <c r="A7" s="6"/>
       <c r="B7" s="18"/>
       <c r="C7" s="19"/>
@@ -1773,7 +1794,7 @@
       <c r="E7" s="3"/>
       <c r="F7" s="5"/>
     </row>
-    <row r="8" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="17.100000000000001" customHeight="1">
       <c r="A8" s="6"/>
       <c r="B8" s="18"/>
       <c r="C8" s="19"/>
@@ -1781,7 +1802,7 @@
       <c r="E8" s="3"/>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="17.100000000000001" customHeight="1">
       <c r="A9" s="6"/>
       <c r="B9" s="18"/>
       <c r="C9" s="19"/>
@@ -1789,7 +1810,7 @@
       <c r="E9" s="3"/>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" ht="17.100000000000001" customHeight="1">
       <c r="A10" s="6"/>
       <c r="B10" s="18"/>
       <c r="C10" s="19"/>
@@ -1797,7 +1818,7 @@
       <c r="E10" s="3"/>
       <c r="F10" s="5"/>
     </row>
-    <row r="11" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" ht="17.100000000000001" customHeight="1">
       <c r="A11" s="6"/>
       <c r="B11" s="18"/>
       <c r="C11" s="19"/>
@@ -1805,7 +1826,7 @@
       <c r="E11" s="3"/>
       <c r="F11" s="5"/>
     </row>
-    <row r="12" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" ht="17.100000000000001" customHeight="1">
       <c r="A12" s="6"/>
       <c r="B12" s="18"/>
       <c r="C12" s="19"/>
@@ -1813,7 +1834,7 @@
       <c r="E12" s="3"/>
       <c r="F12" s="5"/>
     </row>
-    <row r="13" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" ht="17.100000000000001" customHeight="1">
       <c r="A13" s="6"/>
       <c r="B13" s="18"/>
       <c r="C13" s="19"/>
@@ -1821,7 +1842,7 @@
       <c r="E13" s="3"/>
       <c r="F13" s="5"/>
     </row>
-    <row r="14" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" ht="17.100000000000001" customHeight="1">
       <c r="A14" s="6"/>
       <c r="B14" s="18"/>
       <c r="C14" s="19"/>
@@ -1829,7 +1850,7 @@
       <c r="E14" s="3"/>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" ht="17.100000000000001" customHeight="1">
       <c r="A15" s="6"/>
       <c r="B15" s="18"/>
       <c r="C15" s="19"/>
@@ -1837,7 +1858,7 @@
       <c r="E15" s="3"/>
       <c r="F15" s="5"/>
     </row>
-    <row r="16" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" ht="17.100000000000001" customHeight="1">
       <c r="A16" s="6"/>
       <c r="B16" s="18"/>
       <c r="C16" s="19"/>
@@ -1845,7 +1866,7 @@
       <c r="E16" s="3"/>
       <c r="F16" s="5"/>
     </row>
-    <row r="17" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" ht="17.100000000000001" customHeight="1">
       <c r="A17" s="6"/>
       <c r="B17" s="18"/>
       <c r="C17" s="19"/>
@@ -1853,7 +1874,7 @@
       <c r="E17" s="3"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" ht="17.100000000000001" customHeight="1">
       <c r="A18" s="6"/>
       <c r="B18" s="18"/>
       <c r="C18" s="19"/>
@@ -1861,7 +1882,7 @@
       <c r="E18" s="3"/>
       <c r="F18" s="5"/>
     </row>
-    <row r="19" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" ht="17.100000000000001" customHeight="1">
       <c r="A19" s="6"/>
       <c r="B19" s="18"/>
       <c r="C19" s="19"/>
@@ -1869,7 +1890,7 @@
       <c r="E19" s="3"/>
       <c r="F19" s="5"/>
     </row>
-    <row r="20" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" ht="17.100000000000001" customHeight="1">
       <c r="A20" s="6"/>
       <c r="B20" s="18"/>
       <c r="C20" s="19"/>
@@ -1877,7 +1898,7 @@
       <c r="E20" s="3"/>
       <c r="F20" s="5"/>
     </row>
-    <row r="21" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" ht="17.100000000000001" customHeight="1">
       <c r="A21" s="6"/>
       <c r="B21" s="18"/>
       <c r="C21" s="19"/>
@@ -1885,7 +1906,7 @@
       <c r="E21" s="3"/>
       <c r="F21" s="5"/>
     </row>
-    <row r="22" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" ht="17.100000000000001" customHeight="1">
       <c r="A22" s="6"/>
       <c r="B22" s="18"/>
       <c r="C22" s="19"/>
@@ -1893,7 +1914,7 @@
       <c r="E22" s="3"/>
       <c r="F22" s="5"/>
     </row>
-    <row r="23" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" ht="17.100000000000001" customHeight="1">
       <c r="A23" s="6"/>
       <c r="B23" s="18"/>
       <c r="C23" s="19"/>
@@ -1901,7 +1922,7 @@
       <c r="E23" s="3"/>
       <c r="F23" s="5"/>
     </row>
-    <row r="24" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" ht="17.100000000000001" customHeight="1">
       <c r="A24" s="6"/>
       <c r="B24" s="18"/>
       <c r="C24" s="19"/>
@@ -1909,7 +1930,7 @@
       <c r="E24" s="3"/>
       <c r="F24" s="5"/>
     </row>
-    <row r="25" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" ht="17.100000000000001" customHeight="1">
       <c r="A25" s="6"/>
       <c r="B25" s="18"/>
       <c r="C25" s="19"/>
@@ -1917,7 +1938,7 @@
       <c r="E25" s="3"/>
       <c r="F25" s="5"/>
     </row>
-    <row r="26" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" ht="17.100000000000001" customHeight="1">
       <c r="A26" s="6"/>
       <c r="B26" s="18"/>
       <c r="C26" s="19"/>
@@ -1925,7 +1946,7 @@
       <c r="E26" s="3"/>
       <c r="F26" s="5"/>
     </row>
-    <row r="27" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" ht="17.100000000000001" customHeight="1">
       <c r="A27" s="6"/>
       <c r="B27" s="18"/>
       <c r="C27" s="19"/>
@@ -1933,7 +1954,7 @@
       <c r="E27" s="3"/>
       <c r="F27" s="5"/>
     </row>
-    <row r="28" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" ht="17.100000000000001" customHeight="1">
       <c r="A28" s="6"/>
       <c r="B28" s="18"/>
       <c r="C28" s="19"/>
@@ -1941,7 +1962,7 @@
       <c r="E28" s="3"/>
       <c r="F28" s="5"/>
     </row>
-    <row r="29" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" ht="15.95" customHeight="1">
       <c r="A29" s="12"/>
       <c r="B29" s="13"/>
       <c r="C29" s="13"/>
@@ -1949,20 +1970,20 @@
       <c r="E29" s="4"/>
       <c r="F29" s="5"/>
     </row>
-    <row r="30" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" ht="15.95" customHeight="1">
       <c r="A30" s="14" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B30" s="15">
         <f>SUM(B4:B28)</f>
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
       <c r="F30" s="5"/>
     </row>
-    <row r="31" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" ht="15.95" customHeight="1">
       <c r="A31" s="7"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -1970,7 +1991,7 @@
       <c r="E31" s="4"/>
       <c r="F31" s="5"/>
     </row>
-    <row r="32" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" ht="15.95" customHeight="1">
       <c r="A32" s="7"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -1978,7 +1999,7 @@
       <c r="E32" s="4"/>
       <c r="F32" s="5"/>
     </row>
-    <row r="33" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" ht="15.95" customHeight="1">
       <c r="A33" s="8"/>
       <c r="B33" s="9"/>
       <c r="C33" s="9"/>

</xml_diff>

<commit_message>
:sparkles::pencil: Fixed player spawning & Docs updated
</commit_message>
<xml_diff>
--- a/docs/DTT-Test-Hour-Log-1.xlsx
+++ b/docs/DTT-Test-Hour-Log-1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Mazes-for-days\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21E3D882-A776-4890-8C12-B622FA7321B8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1783543E-E5CB-4216-A55A-95A43BF91645}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="555" yWindow="4290" windowWidth="36690" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DTT Test Hour Log" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Subject</t>
   </si>
@@ -86,6 +86,12 @@
   </si>
   <si>
     <t>Made Quick and dirty test Prefabs and also started to make some extra assets</t>
+  </si>
+  <si>
+    <t>Implemented Shader &amp; new Walls</t>
+  </si>
+  <si>
+    <t>Implemented new walls made in blende &amp; made Cell shaded Shader</t>
   </si>
 </sst>
 </file>
@@ -1691,7 +1697,7 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.5" defaultRowHeight="15" customHeight="1"/>
@@ -1746,7 +1752,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="19">
-        <v>43952</v>
+        <v>43976</v>
       </c>
       <c r="D4" s="16" t="s">
         <v>7</v>
@@ -1762,7 +1768,7 @@
         <v>0.5</v>
       </c>
       <c r="C5" s="19">
-        <v>43952</v>
+        <v>43977</v>
       </c>
       <c r="D5" s="16" t="s">
         <v>9</v>
@@ -1778,7 +1784,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="19">
-        <v>43952</v>
+        <v>43977</v>
       </c>
       <c r="D6" s="16" t="s">
         <v>11</v>
@@ -1787,10 +1793,18 @@
       <c r="F6" s="5"/>
     </row>
     <row r="7" spans="1:6" ht="17.100000000000001" customHeight="1">
-      <c r="A7" s="6"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="16"/>
+      <c r="A7" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="18">
+        <v>3</v>
+      </c>
+      <c r="C7" s="19">
+        <v>43983</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>13</v>
+      </c>
       <c r="E7" s="3"/>
       <c r="F7" s="5"/>
     </row>
@@ -1976,7 +1990,7 @@
       </c>
       <c r="B30" s="15">
         <f>SUM(B4:B28)</f>
-        <v>3.5</v>
+        <v>6.5</v>
       </c>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>

</xml_diff>

<commit_message>
:sparkles: Added Shader toggle & more walls
</commit_message>
<xml_diff>
--- a/docs/DTT-Test-Hour-Log-1.xlsx
+++ b/docs/DTT-Test-Hour-Log-1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Mazes-for-days\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1783543E-E5CB-4216-A55A-95A43BF91645}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{732BFE49-9069-4DF9-9F80-46F253E610DF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="1560" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Subject</t>
   </si>
@@ -92,6 +92,30 @@
   </si>
   <si>
     <t>Implemented new walls made in blende &amp; made Cell shaded Shader</t>
+  </si>
+  <si>
+    <t>Implemented Shader Toggle</t>
+  </si>
+  <si>
+    <t>Implemented Shader toggle to switch between custom shader &amp; default URP</t>
+  </si>
+  <si>
+    <t>Animated Small menu &amp; added extra Walls</t>
+  </si>
+  <si>
+    <t>Added menu animations &amp; added more walls variants</t>
+  </si>
+  <si>
+    <t>Made Documentation</t>
+  </si>
+  <si>
+    <t>Used doxygen for documentation page and made UML Diagrams</t>
+  </si>
+  <si>
+    <t>Bug Fixes</t>
+  </si>
+  <si>
+    <t>fixed some background calculation bugs</t>
   </si>
 </sst>
 </file>
@@ -1696,8 +1720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.5" defaultRowHeight="15" customHeight="1"/>
@@ -1744,12 +1768,12 @@
       <c r="E3" s="3"/>
       <c r="F3" s="5"/>
     </row>
-    <row r="4" spans="1:6" ht="17.100000000000001" customHeight="1">
+    <row r="4" spans="1:6" ht="16.5" customHeight="1">
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="18">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C4" s="19">
         <v>43976</v>
@@ -1809,34 +1833,66 @@
       <c r="F7" s="5"/>
     </row>
     <row r="8" spans="1:6" ht="17.100000000000001" customHeight="1">
-      <c r="A8" s="6"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="16"/>
+      <c r="A8" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="18">
+        <v>1</v>
+      </c>
+      <c r="C8" s="19">
+        <v>43988</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>15</v>
+      </c>
       <c r="E8" s="3"/>
       <c r="F8" s="5"/>
     </row>
     <row r="9" spans="1:6" ht="17.100000000000001" customHeight="1">
-      <c r="A9" s="6"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="16"/>
+      <c r="A9" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="18">
+        <v>1</v>
+      </c>
+      <c r="C9" s="19">
+        <v>43988</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>17</v>
+      </c>
       <c r="E9" s="3"/>
       <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:6" ht="17.100000000000001" customHeight="1">
-      <c r="A10" s="6"/>
-      <c r="B10" s="18"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="16"/>
+      <c r="A10" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="18">
+        <v>1</v>
+      </c>
+      <c r="C10" s="19">
+        <v>43988</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>19</v>
+      </c>
       <c r="E10" s="3"/>
       <c r="F10" s="5"/>
     </row>
     <row r="11" spans="1:6" ht="17.100000000000001" customHeight="1">
-      <c r="A11" s="6"/>
-      <c r="B11" s="18"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="16"/>
+      <c r="A11" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="18">
+        <v>1</v>
+      </c>
+      <c r="C11" s="19">
+        <v>43988</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>21</v>
+      </c>
       <c r="E11" s="3"/>
       <c r="F11" s="5"/>
     </row>
@@ -1990,7 +2046,7 @@
       </c>
       <c r="B30" s="15">
         <f>SUM(B4:B28)</f>
-        <v>6.5</v>
+        <v>12.5</v>
       </c>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>

</xml_diff>

<commit_message>
:pencil: Last doc update
</commit_message>
<xml_diff>
--- a/docs/DTT-Test-Hour-Log-1.xlsx
+++ b/docs/DTT-Test-Hour-Log-1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Mazes-for-days\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{732BFE49-9069-4DF9-9F80-46F253E610DF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBA618E7-913F-47B2-9E33-14CC8D54C707}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="1560" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,6 +28,84 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Kevin Celinski</author>
+  </authors>
+  <commentList>
+    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{92C5FC76-0EDA-4831-9CB7-8847FC09E473}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Kevin Celinski:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+http://weblog.jamisbuck.org/2011/1/24/maze-generation-hunt-and-kill-algorithm i</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>s used as reference but the original is not written in C#</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D7" authorId="0" shapeId="0" xr:uid="{C6475091-482B-44EE-B4FB-2E71089A77E0}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Kevin Celinski:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+https://connect.unity.com/p/zelda-inspired-toon-shading-in-shadergraph </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>is referenced</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -125,7 +203,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="13">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -188,6 +266,26 @@
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1717,11 +1815,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.5" defaultRowHeight="15" customHeight="1"/>
@@ -1752,7 +1850,7 @@
       <c r="E2" s="22"/>
       <c r="F2" s="23"/>
     </row>
-    <row r="3" spans="1:6" ht="17.100000000000001" customHeight="1">
+    <row r="3" spans="1:6" ht="16.5" customHeight="1">
       <c r="A3" s="17" t="s">
         <v>0</v>
       </c>
@@ -2088,5 +2186,6 @@
     <oddFooter>&amp;L&amp;"Helvetica,Regular"&amp;12&amp;K000000	&amp;P</oddFooter>
   </headerFooter>
   <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>